<commit_message>
added support for lowercase indexing
</commit_message>
<xml_diff>
--- a/examples/1536_well_simple.xlsx
+++ b/examples/1536_well_simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholas/Code/plate-chain/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abelgurung/Desktop/project/microplateParser/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B190207-CAD9-DD43-86F2-66EFABAE2CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2144AC-A373-5E4C-AF68-030D37DD77C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37560" yWindow="2560" windowWidth="28040" windowHeight="17440" xr2:uid="{57F97038-01F2-AB4E-87CA-8245C61FFD1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19460" xr2:uid="{57F97038-01F2-AB4E-87CA-8245C61FFD1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="80">
   <si>
     <t>A</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t>SB-048</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AF</t>
   </si>
 </sst>
 </file>
@@ -641,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDA4622-CEC1-FC48-85A1-10F32F294C12}">
-  <dimension ref="A2:AW32"/>
+  <dimension ref="A2:AW34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AH34" sqref="AH34"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5266,6 +5272,304 @@
         <v>77</v>
       </c>
     </row>
+    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" t="s">
+        <v>26</v>
+      </c>
+      <c r="O33" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>29</v>
+      </c>
+      <c r="R33" t="s">
+        <v>30</v>
+      </c>
+      <c r="S33" t="s">
+        <v>31</v>
+      </c>
+      <c r="T33" t="s">
+        <v>32</v>
+      </c>
+      <c r="U33" t="s">
+        <v>33</v>
+      </c>
+      <c r="V33" t="s">
+        <v>34</v>
+      </c>
+      <c r="W33" t="s">
+        <v>35</v>
+      </c>
+      <c r="X33" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>74</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" t="s">
+        <v>26</v>
+      </c>
+      <c r="O34" t="s">
+        <v>27</v>
+      </c>
+      <c r="P34" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>29</v>
+      </c>
+      <c r="R34" t="s">
+        <v>30</v>
+      </c>
+      <c r="S34" t="s">
+        <v>31</v>
+      </c>
+      <c r="T34" t="s">
+        <v>32</v>
+      </c>
+      <c r="U34" t="s">
+        <v>33</v>
+      </c>
+      <c r="V34" t="s">
+        <v>34</v>
+      </c>
+      <c r="W34" t="s">
+        <v>35</v>
+      </c>
+      <c r="X34" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ34" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR34" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>74</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW34" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>